<commit_message>
Vercel Ready Version with styling
</commit_message>
<xml_diff>
--- a/static/data/holidays.xlsx
+++ b/static/data/holidays.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7510"/>
+    <workbookView windowWidth="9600" windowHeight="7520"/>
   </bookViews>
   <sheets>
     <sheet name="Holidays" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -165,18 +165,6 @@
   </si>
   <si>
     <t>CHRISTMAS</t>
-  </si>
-  <si>
-    <t>15.07.2025</t>
-  </si>
-  <si>
-    <t>Shift</t>
-  </si>
-  <si>
-    <t>17.07.2025</t>
-  </si>
-  <si>
-    <t>Band Orr</t>
   </si>
 </sst>
 </file>
@@ -189,14 +177,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -652,148 +633,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1145,10 +1126,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C21" sqref="A21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -1373,28 +1354,6 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" t="s">
-        <v>49</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>